<commit_message>
Added autotests,results and allure-results.
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -165,19 +165,13 @@
     <t>Авторизация корректным логином и корректным паролем с пробелом перед/после пароля</t>
   </si>
   <si>
-    <t>Подскажите, сколько и какх еще устройств необходимо использовать для тестирования для полноты охвата?</t>
-  </si>
-  <si>
     <t>Отсутствует единообразие навигации в смежных разделах. Например, на вкладке "Главная" отсутствует кнопка "Добавить" в разделе "Новости", а в разделе "Претензии" она есть.  В свою очередь, в разделе "Претензии" отсутствует кнопка сортировки, которая есть в разделе "Новости".</t>
   </si>
   <si>
-    <t>Полагаем, что авторизация с пробелом перед/после логина реализована для удобства копирования логина из других приложений, когда часто вместе с символами  логина захватываются т.н. "лишние" пробелы. Это верно?</t>
-  </si>
-  <si>
-    <t>Полагаем, что авторизация с пробелом перед/после пароля реализована для удобства копирования пароля из других приложений, когда часто вместе с символами пароля захватываются т.н. "лишние" пробелы. Это верно?</t>
-  </si>
-  <si>
-    <t>Пишу "пройден", но за последнюю неделю не смог добавить ни одной претензии, хотя вижу, что люди их добавляют. У меня претензия добавлялась более двух недель назад. Сейчас - нет. Что делать в таком случае? ( Проблема именно с претензиями - Новости создаются и отображаются нормально!)</t>
+    <t>Nexus 10 10.05" (2560×1600);Pixel C 9.94"  (2560×1800)</t>
+  </si>
+  <si>
+    <t>Верстка не адаптирована под планшет (альбомный формат), поля растянуты на всю ширины страницы.</t>
   </si>
 </sst>
 </file>
@@ -208,7 +202,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,14 +239,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -453,11 +441,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -492,9 +493,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -507,33 +505,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,7 +860,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -863,7 +875,7 @@
       <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="8" t="s">
         <v>38</v>
       </c>
@@ -876,7 +888,7 @@
       <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
@@ -889,7 +901,7 @@
       <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
@@ -902,7 +914,7 @@
       <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -914,8 +926,8 @@
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
+    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A7" s="25"/>
       <c r="B7" s="10" t="s">
         <v>46</v>
       </c>
@@ -925,12 +937,10 @@
       <c r="D7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
       <c r="B8" s="8" t="s">
         <v>47</v>
       </c>
@@ -940,12 +950,10 @@
       <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>51</v>
-      </c>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -960,7 +968,7 @@
       <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
@@ -973,7 +981,7 @@
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="22"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
@@ -986,7 +994,7 @@
       <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="22"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="8" t="s">
         <v>16</v>
       </c>
@@ -999,7 +1007,7 @@
       <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="22"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1012,7 +1020,7 @@
       <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="22"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="8" t="s">
         <v>18</v>
       </c>
@@ -1027,14 +1035,14 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="22"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="20"/>
     </row>
-    <row r="16" spans="1:5" ht="76" x14ac:dyDescent="0.35">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1046,12 +1054,10 @@
       <c r="D16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>52</v>
-      </c>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="22"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
@@ -1064,7 +1070,7 @@
       <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="8" t="s">
         <v>23</v>
       </c>
@@ -1077,7 +1083,7 @@
       <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="22"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
@@ -1090,7 +1096,7 @@
       <c r="E19" s="20"/>
     </row>
     <row r="20" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A20" s="22"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="8" t="s">
         <v>25</v>
       </c>
@@ -1103,7 +1109,7 @@
       <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A21" s="22"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="8" t="s">
         <v>26</v>
       </c>
@@ -1116,7 +1122,7 @@
       <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="22"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="8" t="s">
         <v>27</v>
       </c>
@@ -1129,7 +1135,7 @@
       <c r="E22" s="20"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="22"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="8" t="s">
         <v>28</v>
       </c>
@@ -1142,25 +1148,29 @@
       <c r="E23" s="20"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="20"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
-      <c r="B25" s="8"/>
+      <c r="A25" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="C25" s="8" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>6</v>
@@ -1168,11 +1178,9 @@
       <c r="E25" s="20"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>42</v>
+      <c r="A26" s="25"/>
+      <c r="B26" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>14</v>
@@ -1180,51 +1188,59 @@
       <c r="D26" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="20"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="22"/>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:5" ht="162.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="25"/>
       <c r="B27" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" ht="162.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="22"/>
-      <c r="B28" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="25"/>
+      <c r="B28" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="22"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="25" x14ac:dyDescent="0.35">
-      <c r="A30" s="22" t="s">
+      <c r="E28" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A29" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>32</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A30" s="25"/>
+      <c r="B30" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>14</v>
@@ -1236,220 +1252,204 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A31" s="22"/>
-      <c r="B31" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="9" t="s">
+    <row r="31" spans="1:5" ht="64" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="64" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>49</v>
-      </c>
+      <c r="E31" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="16"/>
+      <c r="E32" s="17"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="18"/>
-      <c r="E33" s="21"/>
+      <c r="A33" s="16"/>
+      <c r="E33" s="17"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
-      <c r="E34" s="21"/>
+      <c r="A34" s="16"/>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="18"/>
-      <c r="E35" s="21"/>
+      <c r="A35" s="16"/>
+      <c r="E35" s="17"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="18"/>
-      <c r="E36" s="21"/>
+      <c r="A36" s="16"/>
+      <c r="E36" s="17"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
-      <c r="E37" s="21"/>
+      <c r="A37" s="16"/>
+      <c r="E37" s="17"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="18"/>
-      <c r="E38" s="21"/>
+      <c r="A38" s="16"/>
+      <c r="E38" s="17"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="18"/>
-      <c r="E39" s="21"/>
+      <c r="A39" s="16"/>
+      <c r="E39" s="17"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="18"/>
-      <c r="E40" s="21"/>
+      <c r="A40" s="16"/>
+      <c r="E40" s="17"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="18"/>
-      <c r="E41" s="21"/>
+      <c r="A41" s="16"/>
+      <c r="E41" s="17"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="18"/>
-      <c r="E42" s="21"/>
+      <c r="A42" s="16"/>
+      <c r="E42" s="17"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="18"/>
-      <c r="E43" s="21"/>
+      <c r="A43" s="16"/>
+      <c r="E43" s="17"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="18"/>
-      <c r="E44" s="21"/>
+      <c r="A44" s="16"/>
+      <c r="E44" s="17"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="18"/>
-      <c r="E45" s="21"/>
+      <c r="A45" s="16"/>
+      <c r="E45" s="17"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="18"/>
-      <c r="E46" s="21"/>
+      <c r="A46" s="16"/>
+      <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="18"/>
-      <c r="E47" s="21"/>
+      <c r="A47" s="16"/>
+      <c r="E47" s="17"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="18"/>
-      <c r="E48" s="21"/>
+      <c r="A48" s="16"/>
+      <c r="E48" s="17"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="18"/>
-      <c r="E49" s="21"/>
+      <c r="A49" s="16"/>
+      <c r="E49" s="17"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="18"/>
-      <c r="E50" s="21"/>
+      <c r="A50" s="16"/>
+      <c r="E50" s="17"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="18"/>
-      <c r="E51" s="21"/>
+      <c r="A51" s="16"/>
+      <c r="E51" s="17"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="18"/>
-      <c r="E52" s="21"/>
+      <c r="A52" s="16"/>
+      <c r="E52" s="17"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
-      <c r="E53" s="21"/>
+      <c r="A53" s="16"/>
+      <c r="E53" s="17"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="18"/>
-      <c r="E54" s="21"/>
+      <c r="A54" s="16"/>
+      <c r="E54" s="17"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="18"/>
-      <c r="E55" s="21"/>
+      <c r="A55" s="16"/>
+      <c r="E55" s="17"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="18"/>
-      <c r="E56" s="21"/>
+      <c r="A56" s="16"/>
+      <c r="E56" s="17"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="18"/>
-      <c r="E57" s="21"/>
+      <c r="A57" s="16"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="18"/>
-      <c r="E58" s="21"/>
+      <c r="A58" s="16"/>
+      <c r="E58" s="17"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="18"/>
-      <c r="E59" s="21"/>
+      <c r="A59" s="16"/>
+      <c r="E59" s="17"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="18"/>
-      <c r="E60" s="21"/>
+      <c r="A60" s="16"/>
+      <c r="E60" s="17"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="18"/>
-      <c r="E61" s="21"/>
+      <c r="A61" s="16"/>
+      <c r="E61" s="17"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="18"/>
-      <c r="E62" s="21"/>
+      <c r="A62" s="16"/>
+      <c r="E62" s="17"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="18"/>
-      <c r="E63" s="21"/>
+      <c r="A63" s="16"/>
+      <c r="E63" s="17"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="18"/>
-      <c r="E64" s="21"/>
+      <c r="A64" s="16"/>
+      <c r="E64" s="17"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="18"/>
-      <c r="E65" s="21"/>
+      <c r="A65" s="16"/>
+      <c r="E65" s="17"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="18"/>
-      <c r="E66" s="21"/>
+      <c r="A66" s="16"/>
+      <c r="E66" s="17"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="18"/>
-      <c r="E67" s="21"/>
+      <c r="A67" s="16"/>
+      <c r="E67" s="17"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="18"/>
-      <c r="E68" s="21"/>
+      <c r="A68" s="16"/>
+      <c r="E68" s="17"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="18"/>
-      <c r="E69" s="21"/>
+      <c r="A69" s="16"/>
+      <c r="E69" s="17"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="18"/>
-      <c r="E70" s="21"/>
+      <c r="A70" s="16"/>
+      <c r="E70" s="17"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="18"/>
-      <c r="E71" s="21"/>
+      <c r="A71" s="16"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="18"/>
+      <c r="A72" s="16"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="18"/>
+      <c r="A73" s="16"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="18"/>
+      <c r="A74" s="16"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="18"/>
+      <c r="A75" s="16"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="18"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="18"/>
+      <c r="A76" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A30:A31"/>
+  <mergeCells count="5">
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A16:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A25:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>